<commit_message>
financial KPI's (Umsatz, Ertrag per user category)
</commit_message>
<xml_diff>
--- a/graphics/KPI-Overview/Finance-KPIs.xlsx
+++ b/graphics/KPI-Overview/Finance-KPIs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="180" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1220" yWindow="6400" windowWidth="25820" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Umsatz</t>
-  </si>
-  <si>
     <t>Umsatz gesamt</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Verteilung der Verkäufe</t>
+  </si>
+  <si>
+    <t>Ertrag</t>
   </si>
 </sst>
 </file>
@@ -71,9 +71,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0\ &quot;€&quot;;[Red]#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -105,16 +105,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -122,8 +158,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -133,25 +218,173 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="27">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,183 +714,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="5" ySplit="12" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:11">
+      <c r="B1" s="63"/>
+      <c r="C1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="30"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="B2" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="K2" s="30"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="B3" s="63"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2"/>
+      <c r="B4" s="64">
+        <f>SUM(C4:J4)</f>
+        <v>217000</v>
+      </c>
+      <c r="C4" s="38">
+        <v>200000</v>
+      </c>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40">
+        <v>15000</v>
+      </c>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43">
+        <v>1000</v>
+      </c>
+      <c r="I4" s="44"/>
+      <c r="J4" s="45">
+        <v>1000</v>
+      </c>
+      <c r="K4" s="46"/>
     </row>
-    <row r="2" spans="1:10">
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1">
-        <v>300000</v>
-      </c>
-      <c r="C4">
-        <v>100000</v>
-      </c>
-      <c r="E4">
-        <v>200000</v>
-      </c>
-      <c r="G4">
-        <v>1000</v>
-      </c>
-      <c r="I4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="65"/>
+      <c r="C5" s="37">
+        <v>0.06</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="47">
+        <v>0.15</v>
+      </c>
+      <c r="F5" s="48"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="50">
+        <v>0.12</v>
+      </c>
+      <c r="I5" s="51"/>
+      <c r="J5" s="52">
+        <v>0.05</v>
+      </c>
+      <c r="K5" s="53"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="27">
+        <v>300</v>
+      </c>
+      <c r="D6" s="28">
+        <v>5000</v>
+      </c>
+      <c r="E6" s="18">
+        <v>100</v>
+      </c>
+      <c r="F6" s="19">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="20">
+        <v>100000</v>
+      </c>
+      <c r="H6" s="7">
+        <v>30000</v>
+      </c>
+      <c r="I6" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="J6" s="35">
         <v>500</v>
       </c>
-      <c r="D5">
-        <v>5000</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G5" s="1">
-        <v>30000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>5000000</v>
-      </c>
-      <c r="I5" s="1">
-        <v>500</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="K6" s="36">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="63"/>
+      <c r="C7" s="25">
+        <v>0.99</v>
+      </c>
+      <c r="D7" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="G7" s="17">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="J7" s="33">
+        <v>0.4</v>
+      </c>
+      <c r="K7" s="34">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" thickBot="1">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="66">
+        <f>SUM(C8:K8)</f>
+        <v>187175000</v>
+      </c>
+      <c r="C8" s="27">
+        <f>C4*C7*C6</f>
+        <v>59400000</v>
+      </c>
+      <c r="D8" s="28">
+        <f>C4*D6*D7</f>
+        <v>10000000</v>
+      </c>
+      <c r="E8" s="18">
+        <f>E4*E7*E6</f>
+        <v>1200000</v>
+      </c>
+      <c r="F8" s="19">
+        <f>E4*F6*F7</f>
+        <v>29925000</v>
+      </c>
+      <c r="G8" s="20">
+        <f>E4*G6*G7</f>
+        <v>750000</v>
+      </c>
+      <c r="H8" s="7">
+        <f>H4*H7*H6</f>
+        <v>29700000</v>
+      </c>
+      <c r="I8" s="8">
+        <f>H4*I6*I7</f>
+        <v>50000000</v>
+      </c>
+      <c r="J8" s="35">
+        <f>J4*J7*J6</f>
+        <v>200000</v>
+      </c>
+      <c r="K8" s="36">
+        <f>J4*K6*K7</f>
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" thickTop="1">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.6</v>
+      <c r="B9" s="67">
+        <f>SUM(C9:K9)</f>
+        <v>18819250</v>
+      </c>
+      <c r="C9" s="54">
+        <f>C8*C5</f>
+        <v>3564000</v>
+      </c>
+      <c r="D9" s="55">
+        <f>D8*C5</f>
+        <v>600000</v>
+      </c>
+      <c r="E9" s="56">
+        <f>E8*E5</f>
+        <v>180000</v>
+      </c>
+      <c r="F9" s="57">
+        <f>F8*E5</f>
+        <v>4488750</v>
+      </c>
+      <c r="G9" s="58">
+        <f>G8*E5</f>
+        <v>112500</v>
+      </c>
+      <c r="H9" s="59">
+        <f>H8*H5</f>
+        <v>3564000</v>
+      </c>
+      <c r="I9" s="60">
+        <f>I8*H5</f>
+        <v>6000000</v>
+      </c>
+      <c r="J9" s="61">
+        <f>J8*J5</f>
+        <v>10000</v>
+      </c>
+      <c r="K9" s="62">
+        <f>K8*J5</f>
+        <v>300000</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4">
-        <f>C4*C6*C5</f>
-        <v>49000000</v>
-      </c>
-      <c r="D7" s="4">
-        <f>C4*D5*D6</f>
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.06</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.12</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
+    <row r="10" spans="1:11">
+      <c r="B10" s="63"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="15">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
updated finance (xlsx) and portrait
</commit_message>
<xml_diff>
--- a/graphics/KPI-Overview/Finance-KPIs.xlsx
+++ b/graphics/KPI-Overview/Finance-KPIs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="6400" windowWidth="25820" windowHeight="13460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Umsatz gesamt</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Ertrag</t>
+  </si>
+  <si>
+    <t>Ertrag/Mitarbeiter</t>
+  </si>
+  <si>
+    <t>Umsatz/Mitarbeiter</t>
+  </si>
+  <si>
+    <t># Mitarbeiter (intern, fest)</t>
+  </si>
+  <si>
+    <t>Mitarbeitertage Fremdleistung</t>
+  </si>
+  <si>
+    <t>entspricht externe MA</t>
   </si>
 </sst>
 </file>
@@ -237,29 +252,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -269,24 +269,12 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -294,54 +282,6 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -357,6 +297,82 @@
     <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -714,18 +730,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="5" ySplit="12" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
@@ -738,138 +754,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="B1" s="63"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="61"/>
+      <c r="E1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="1" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="29" t="s">
+      <c r="I1" s="66"/>
+      <c r="J1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="30"/>
+      <c r="K1" s="68"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="29" t="s">
+      <c r="I2" s="66"/>
+      <c r="J2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="30"/>
+      <c r="K2" s="68"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="63"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="64">
+      <c r="B4" s="39">
         <f>SUM(C4:J4)</f>
         <v>217000</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="44">
         <v>200000</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40">
+      <c r="D4" s="45"/>
+      <c r="E4" s="46">
         <v>15000</v>
       </c>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="43">
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="49">
         <v>1000</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45">
+      <c r="I4" s="50"/>
+      <c r="J4" s="51">
         <v>1000</v>
       </c>
-      <c r="K4" s="46"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="37">
+      <c r="B5" s="40"/>
+      <c r="C5" s="28">
         <v>0.06</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="47">
+      <c r="D5" s="17"/>
+      <c r="E5" s="53">
         <v>0.15</v>
       </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="50">
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="56">
         <v>0.12</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52">
+      <c r="I5" s="57"/>
+      <c r="J5" s="58">
         <v>0.05</v>
       </c>
-      <c r="K5" s="53"/>
+      <c r="K5" s="59"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="27">
+      <c r="B6" s="38"/>
+      <c r="C6" s="20">
         <v>300</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="21">
         <v>5000</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="13">
         <v>100</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="14">
         <v>10000</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="15">
         <v>100000</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>30000</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <v>5000000</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="26">
         <v>500</v>
       </c>
-      <c r="K6" s="36">
+      <c r="K6" s="27">
         <v>10000</v>
       </c>
     </row>
@@ -877,32 +893,32 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="25">
+      <c r="B7" s="38"/>
+      <c r="C7" s="18">
         <v>0.99</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="19">
         <v>0.01</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="10">
         <v>0.8</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="11">
         <v>0.19950000000000001</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="12">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>0.99</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="4">
         <v>0.01</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="24">
         <v>0.4</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="25">
         <v>0.6</v>
       </c>
     </row>
@@ -910,43 +926,43 @@
       <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="66">
+      <c r="B8" s="41">
         <f>SUM(C8:K8)</f>
         <v>187175000</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="20">
         <f>C4*C7*C6</f>
         <v>59400000</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="21">
         <f>C4*D6*D7</f>
         <v>10000000</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="13">
         <f>E4*E7*E6</f>
         <v>1200000</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="14">
         <f>E4*F6*F7</f>
         <v>29925000</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="15">
         <f>E4*G6*G7</f>
         <v>750000</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <f>H4*H7*H6</f>
         <v>29700000</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="6">
         <f>H4*I6*I7</f>
         <v>50000000</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="26">
         <f>J4*J7*J6</f>
         <v>200000</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8" s="27">
         <f>J4*K6*K7</f>
         <v>6000000</v>
       </c>
@@ -955,68 +971,104 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="67">
+      <c r="B9" s="42">
         <f>SUM(C9:K9)</f>
         <v>18819250</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="29">
         <f>C8*C5</f>
         <v>3564000</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="30">
         <f>D8*C5</f>
         <v>600000</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="31">
         <f>E8*E5</f>
         <v>180000</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="32">
         <f>F8*E5</f>
         <v>4488750</v>
       </c>
-      <c r="G9" s="58">
+      <c r="G9" s="33">
         <f>G8*E5</f>
         <v>112500</v>
       </c>
-      <c r="H9" s="59">
+      <c r="H9" s="34">
         <f>H8*H5</f>
         <v>3564000</v>
       </c>
-      <c r="I9" s="60">
+      <c r="I9" s="35">
         <f>I8*H5</f>
         <v>6000000</v>
       </c>
-      <c r="J9" s="61">
+      <c r="J9" s="36">
         <f>J8*J5</f>
         <v>10000</v>
       </c>
-      <c r="K9" s="62">
+      <c r="K9" s="37">
         <f>K8*J5</f>
         <v>300000</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="B10" s="63"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="69">
+        <f>B9/B11</f>
+        <v>55350.73529411765</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="69">
+        <f>B8/B11</f>
+        <v>550514.70588235289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>95000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <f>B15/200</f>
+        <v>475</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:I2"/>
@@ -1025,6 +1077,13 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>